<commit_message>
Added instructions in creating vm
</commit_message>
<xml_diff>
--- a/ConfigSheet.xlsx
+++ b/ConfigSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhammadislam/Projects/Documentation/ocp42install/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC35EC46-9612-B14F-AEBF-504E28150D41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4620D65B-FA80-4646-B568-DE63EE18A538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{9D796296-53CE-6841-A684-C4615D6CE825}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Master</t>
   </si>
@@ -88,6 +88,21 @@
   </si>
   <si>
     <t>Number of Worker</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>rhcos-4.2.0-x86_64-vmware-template</t>
+  </si>
+  <si>
+    <t>ocp42-installer-template</t>
+  </si>
+  <si>
+    <t>ocp42-lb-template</t>
+  </si>
+  <si>
+    <t>nfs-server-template</t>
   </si>
 </sst>
 </file>
@@ -442,20 +457,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293B764B-F9F4-4945-9939-C6CDB1EBE02B}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:F16"/>
+      <selection activeCell="G8" sqref="A1:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="16.6640625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="35.6640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -474,8 +491,11 @@
       <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,8 +511,11 @@
       <c r="E2" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -508,8 +531,11 @@
       <c r="E3" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -528,8 +554,11 @@
       <c r="F4" s="1">
         <v>500</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -545,8 +574,11 @@
       <c r="E5" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -562,8 +594,11 @@
       <c r="E6" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -579,8 +614,11 @@
       <c r="E7" s="1">
         <v>120</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -596,8 +634,11 @@
       <c r="E8" s="1">
         <v>500</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -617,7 +658,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -634,7 +675,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -642,7 +683,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -650,7 +691,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -658,7 +699,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>